<commit_message>
One more customer added in add customer test case test data
</commit_message>
<xml_diff>
--- a/DataDriven/src/test/resources/excel/testdata.xlsx
+++ b/DataDriven/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java11Automation\DataDrivenFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationFramework\DataDriven\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3667FDE-F7F5-455B-9BA6-928649C1DDBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64863D60-5616-4AC0-8CE4-08ADC20A11C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{4EE8F7EA-477F-4DEF-A3DC-0173AE102C5D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4EE8F7EA-477F-4DEF-A3DC-0173AE102C5D}"/>
   </bookViews>
   <sheets>
     <sheet name="doLogin" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>username</t>
   </si>
@@ -493,10 +493,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF08070-7C98-49AC-A4CF-D93977297943}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,6 +543,17 @@
       </c>
       <c r="C4">
         <v>23343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>3456</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4E9E07-9EC1-4762-9166-BB4B61AD55FE}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>